<commit_message>
update Excel with modified requirement 6.2
</commit_message>
<xml_diff>
--- a/documents/WDSF scrutiny software certification.xlsx
+++ b/documents/WDSF scrutiny software certification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Dev\WDSF-Competition-Software-Certification\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB484694-0AF3-4BC3-8E8F-76DA77422D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0EC5C0-9116-4A79-A66D-C89E9C2CCF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24000" yWindow="1572" windowWidth="22044" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements PC" sheetId="1" r:id="rId1"/>
@@ -487,9 +487,6 @@
     <t>The software should be aware that the number of components might change (for example in lower classes the choreography might not be judges)</t>
   </si>
   <si>
-    <t>The software should be able to write the relevant data (judges, couples, heats) in the format used by the official WDSF judging software. For information on the format please see  https://bitbucket.org/signalkontor/wdsf-judging-client/wiki/Format_of_data</t>
-  </si>
-  <si>
     <t>New Judging System 2.1</t>
   </si>
   <si>
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>The print out must contain all information neccesary to identify the competition, adjudicator, scrutiny and chairperson without doubt.</t>
+  </si>
+  <si>
+    <t>The software should be able to write the relevant data (couples, heats, scores) in the format used by the WDSF Media Team. https://github.com/jaykay-design/WDSF-Competition-Software-Certification/blob/master/documents/World_Dance_Tree.zip</t>
   </si>
 </sst>
 </file>
@@ -624,9 +624,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -638,6 +635,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,26 +979,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="13"/>
+    <col min="1" max="1" width="11.44140625" style="12"/>
     <col min="2" max="2" width="170.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
@@ -1020,7 +1020,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1031,7 +1031,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1040,7 +1040,7 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1051,7 +1051,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1062,7 +1062,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1073,7 +1073,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1095,7 +1095,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1103,8 +1103,8 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1115,7 +1115,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1125,8 +1125,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>64</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1147,16 +1147,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
         <v>127</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
         <v>128</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1167,7 +1167,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
+      <c r="A24" s="13">
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1175,8 +1175,8 @@
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1186,8 +1186,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1197,8 +1197,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1206,7 +1206,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1216,8 +1216,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1227,8 +1227,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1239,7 +1239,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="15" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1249,8 +1249,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="15" t="s">
         <v>144</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1271,8 +1271,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
         <v>145</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1282,8 +1282,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
         <v>146</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1293,8 +1293,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
         <v>147</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1305,7 +1305,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="15" t="s">
         <v>148</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1316,23 +1316,23 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="16">
+      <c r="A38" s="15">
         <v>3.14</v>
       </c>
       <c r="B38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="15"/>
+      <c r="B39" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" t="s">
-        <v>159</v>
-      </c>
       <c r="C39" s="8"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>4</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1341,7 +1341,7 @@
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1351,8 +1351,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -1362,8 +1362,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
         <v>123</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="14">
+      <c r="A48" s="13">
         <v>5</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1382,8 +1382,8 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1393,8 +1393,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="16" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -1404,8 +1404,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -1416,7 +1416,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -1426,8 +1426,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -1438,7 +1438,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -1448,8 +1448,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="16" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -1460,7 +1460,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -1470,8 +1470,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -1481,8 +1481,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="16" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -1492,8 +1492,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="16" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
         <v>119</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="15" t="s">
         <v>120</v>
       </c>
       <c r="B60" s="9" t="s">
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="15" t="s">
         <v>125</v>
       </c>
       <c r="B61" s="9" t="s">
@@ -1523,24 +1523,24 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="16">
+      <c r="A62" s="15">
         <v>5.14</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="14">
+      <c r="A64" s="13">
         <v>6</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C64" s="3"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B65" t="s">
@@ -1551,16 +1551,16 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="16">
+      <c r="A66" s="15">
         <v>6.2</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="16">
+      <c r="A67" s="15">
         <v>6.3</v>
       </c>
       <c r="B67" t="s">
@@ -1569,7 +1569,7 @@
       <c r="C67" s="8"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="16">
+      <c r="A68" s="15">
         <v>6.4</v>
       </c>
       <c r="B68" t="s">
@@ -1578,7 +1578,7 @@
       <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="16">
+      <c r="A69" s="15">
         <v>6.5</v>
       </c>
       <c r="B69" t="s">
@@ -1587,7 +1587,7 @@
       <c r="C69" s="8"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="16">
+      <c r="A70" s="15">
         <v>6.6</v>
       </c>
       <c r="B70" t="s">
@@ -1596,12 +1596,12 @@
       <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="16"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="5"/>
       <c r="C71" s="8"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="14">
+      <c r="A73" s="13">
         <v>7</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -1610,7 +1610,7 @@
       <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="15" t="s">
         <v>90</v>
       </c>
       <c r="B74" s="5" t="s">
@@ -1620,8 +1620,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="16" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="15" t="s">
         <v>91</v>
       </c>
       <c r="B75" s="5" t="s">
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="15" t="s">
         <v>92</v>
       </c>
       <c r="B76" s="5" t="s">
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="15" t="s">
         <v>93</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -1653,8 +1653,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="16" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="15" t="s">
         <v>94</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -1664,8 +1664,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="16" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="15" t="s">
         <v>95</v>
       </c>
       <c r="B79" s="5" t="s">
@@ -1675,8 +1675,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A80" s="16" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B80" s="5" t="s">
@@ -1686,8 +1686,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="16" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B81" s="5" t="s">
@@ -1697,8 +1697,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="16" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="15" t="s">
         <v>98</v>
       </c>
       <c r="B82" s="5" t="s">
@@ -1709,7 +1709,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="15" t="s">
         <v>99</v>
       </c>
       <c r="B83" s="5" t="s">
@@ -1720,7 +1720,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="15" t="s">
         <v>100</v>
       </c>
       <c r="B84" s="5" t="s">
@@ -1730,8 +1730,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="16" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="15" t="s">
         <v>101</v>
       </c>
       <c r="B85" s="5" t="s">
@@ -1741,8 +1741,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="16" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B86" s="5" t="s">
@@ -1752,8 +1752,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="16" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="15" t="s">
         <v>103</v>
       </c>
       <c r="B87" s="5" t="s">
@@ -1763,8 +1763,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="16" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="15" t="s">
         <v>104</v>
       </c>
       <c r="B88" s="5" t="s">
@@ -1774,8 +1774,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="16" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="15" t="s">
         <v>105</v>
       </c>
       <c r="B89" s="5" t="s">
@@ -1785,8 +1785,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="16" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="15" t="s">
         <v>106</v>
       </c>
       <c r="B90" s="5" t="s">
@@ -1796,8 +1796,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="16" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="15" t="s">
         <v>107</v>
       </c>
       <c r="B91" s="5" t="s">
@@ -1807,8 +1807,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="16" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="15" t="s">
         <v>108</v>
       </c>
       <c r="B92" s="5" t="s">
@@ -1818,8 +1818,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="16" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B93" s="5" t="s">
@@ -1829,8 +1829,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A94" s="16" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="15" t="s">
         <v>110</v>
       </c>
       <c r="B94" s="5" t="s">
@@ -1841,7 +1841,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="16" t="s">
+      <c r="A95" s="15" t="s">
         <v>111</v>
       </c>
       <c r="B95" s="10" t="s">
@@ -1852,7 +1852,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="13">
+      <c r="A96" s="12">
         <v>7.23</v>
       </c>
       <c r="B96" t="s">

</xml_diff>